<commit_message>
- Switched to HPCA template. - Re-executed wrong experiments and added revised graphs in paper. - Checked and corrected every number in the paper (Table 1 not updated   yet). - Added CAMEO IDEAL (no caching). Added CAMEO bars in existing graphs.   Cameo reports really bad numbers. Will check for bugs but these numbers   make sense to me. - Added better CAMEO description in related work and building block   breakdown. - Added discussion about CAMEO in results section. - We are slightly over the page limit (a few lines so far) - Fixed some random typos.
</commit_message>
<xml_diff>
--- a/paper/raw_data/revised/new_results/exp02_COUNTER_SIZE.xlsx
+++ b/paper/raw_data/revised/new_results/exp02_COUNTER_SIZE.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aprodrom\Desktop\MemPod\paper\raw_data\revised\new_results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prodr\Desktop\MemPod\paper\raw_data\revised\new_results\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
   <externalReferences>
     <externalReference r:id="rId2"/>
   </externalReferences>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -137,7 +137,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -204,7 +204,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -276,6 +276,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4003-4821-9841-6779AC22DB1B}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -316,6 +321,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-4003-4821-9841-6779AC22DB1B}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -356,6 +366,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-4003-4821-9841-6779AC22DB1B}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -461,6 +476,11 @@
             </c:numRef>
           </c:cat>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-4003-4821-9841-6779AC22DB1B}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -512,7 +532,7 @@
             <c:strRef>
               <c:f>'[1]CTR SIZE (100us)'!$A$42:$A$58</c:f>
               <c:strCache>
-                <c:ptCount val="16"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="3">
                   <c:v>AVG HG</c:v>
                 </c:pt>
@@ -550,6 +570,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-4003-4821-9841-6779AC22DB1B}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
@@ -582,7 +607,7 @@
             <c:strRef>
               <c:f>'[1]CTR SIZE (100us)'!$A$42:$A$58</c:f>
               <c:strCache>
-                <c:ptCount val="16"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="3">
                   <c:v>AVG HG</c:v>
                 </c:pt>
@@ -620,6 +645,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-4003-4821-9841-6779AC22DB1B}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="5"/>
@@ -652,7 +682,7 @@
             <c:strRef>
               <c:f>'[1]CTR SIZE (100us)'!$A$42:$A$58</c:f>
               <c:strCache>
-                <c:ptCount val="16"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="3">
                   <c:v>AVG HG</c:v>
                 </c:pt>
@@ -690,6 +720,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-4003-4821-9841-6779AC22DB1B}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="6"/>
@@ -728,7 +763,7 @@
             <c:strRef>
               <c:f>'[1]CTR SIZE (100us)'!$A$42:$A$58</c:f>
               <c:strCache>
-                <c:ptCount val="16"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="3">
                   <c:v>AVG HG</c:v>
                 </c:pt>
@@ -751,6 +786,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-4003-4821-9841-6779AC22DB1B}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -914,7 +954,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1997,6 +2036,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2032,6 +2088,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2187,7 +2260,7 @@
   <dimension ref="A1:T58"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="AA54" sqref="AA54"/>
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added the alternative results section. Needs work with figures and a macro to make it easy to select one or the other
</commit_message>
<xml_diff>
--- a/paper/raw_data/revised/new_results/exp02_COUNTER_SIZE.xlsx
+++ b/paper/raw_data/revised/new_results/exp02_COUNTER_SIZE.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prodr\Desktop\MemPod\paper\raw_data\revised\new_results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aprodrom\Desktop\MemPod\paper\raw_data\revised\new_results\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <externalReference r:id="rId2"/>
   </externalReferences>
   <calcPr calcId="171027"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -137,7 +138,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -204,7 +205,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -276,7 +277,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-4003-4821-9841-6779AC22DB1B}"/>
             </c:ext>
@@ -321,7 +322,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-4003-4821-9841-6779AC22DB1B}"/>
             </c:ext>
@@ -366,7 +367,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-4003-4821-9841-6779AC22DB1B}"/>
             </c:ext>
@@ -382,8 +383,8 @@
         </c:dLbls>
         <c:gapWidth val="0"/>
         <c:overlap val="94"/>
-        <c:axId val="366277304"/>
-        <c:axId val="366278088"/>
+        <c:axId val="377956480"/>
+        <c:axId val="378003896"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -476,7 +477,7 @@
             </c:numRef>
           </c:cat>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-4003-4821-9841-6779AC22DB1B}"/>
             </c:ext>
@@ -492,8 +493,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="366277304"/>
-        <c:axId val="366278088"/>
+        <c:axId val="377956480"/>
+        <c:axId val="378003896"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -570,7 +571,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-4003-4821-9841-6779AC22DB1B}"/>
             </c:ext>
@@ -645,7 +646,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000005-4003-4821-9841-6779AC22DB1B}"/>
             </c:ext>
@@ -720,7 +721,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000006-4003-4821-9841-6779AC22DB1B}"/>
             </c:ext>
@@ -786,7 +787,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000007-4003-4821-9841-6779AC22DB1B}"/>
             </c:ext>
@@ -802,11 +803,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="366278872"/>
-        <c:axId val="366280440"/>
+        <c:axId val="378103288"/>
+        <c:axId val="378103680"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="366277304"/>
+        <c:axId val="377956480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -902,7 +903,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="366278088"/>
+        <c:crossAx val="378003896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -910,7 +911,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="366278088"/>
+        <c:axId val="378003896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.02"/>
@@ -949,11 +950,12 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US" sz="900" b="1"/>
-                  <a:t>AMMAT / AMMAT(16)</a:t>
+                  <a:t>AMMAT / AMMAT (2)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1008,12 +1010,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="366277304"/>
+        <c:crossAx val="377956480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="366280440"/>
+        <c:axId val="378103680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1104,12 +1106,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="366278872"/>
+        <c:crossAx val="378103288"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="366278872"/>
+        <c:axId val="378103288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1149,7 +1151,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="366280440"/>
+        <c:crossAx val="378103680"/>
         <c:crosses val="max"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2036,23 +2038,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2088,23 +2073,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2260,7 +2228,7 @@
   <dimension ref="A1:T58"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+      <selection activeCell="S44" sqref="S44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>